<commit_message>
Updated scripts to handle new field in create account
</commit_message>
<xml_diff>
--- a/Data Files/Batch/CustomerAndAccountsData.xlsx
+++ b/Data Files/Batch/CustomerAndAccountsData.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cshah\git\nGage-Banking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chintan.shah\git\nGage-Banking\Data Files\Batch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D99139-D373-41F4-8622-91F0DF34AF5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{47FB0726-0CA2-4609-AFDA-BA55CDCA5A34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CustomerData" sheetId="1" r:id="rId1"/>
     <sheet name="AccountData" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="124">
   <si>
     <t>FirstName</t>
   </si>
@@ -102,15 +101,6 @@
     <t>CustomerGroup</t>
   </si>
   <si>
-    <t>Chintan</t>
-  </si>
-  <si>
-    <t>Deepak</t>
-  </si>
-  <si>
-    <t>Shah</t>
-  </si>
-  <si>
     <t>United States of America</t>
   </si>
   <si>
@@ -141,33 +131,15 @@
     <t>English - United States</t>
   </si>
   <si>
-    <t>MID_200001</t>
-  </si>
-  <si>
     <t>Banking Customer</t>
   </si>
   <si>
     <t>09/01/1985</t>
   </si>
   <si>
-    <t>Tushar</t>
-  </si>
-  <si>
-    <t>Khushbu</t>
-  </si>
-  <si>
     <t>11/16/1982</t>
   </si>
   <si>
-    <t>911781001</t>
-  </si>
-  <si>
-    <t>911781000</t>
-  </si>
-  <si>
-    <t>911781002</t>
-  </si>
-  <si>
     <t>03/11/1991</t>
   </si>
   <si>
@@ -192,15 +164,6 @@
     <t>OFFICE</t>
   </si>
   <si>
-    <t>chintan.shah@example.com</t>
-  </si>
-  <si>
-    <t>tushar.shah@example.com</t>
-  </si>
-  <si>
-    <t>khush.shah@example.com</t>
-  </si>
-  <si>
     <t>Home</t>
   </si>
   <si>
@@ -213,21 +176,6 @@
     <t>Text and email</t>
   </si>
   <si>
-    <t>MID_200002</t>
-  </si>
-  <si>
-    <t>MID_200003</t>
-  </si>
-  <si>
-    <t>+17841253545</t>
-  </si>
-  <si>
-    <t>+17841253546</t>
-  </si>
-  <si>
-    <t>+17841253547</t>
-  </si>
-  <si>
     <t>AccTitle</t>
   </si>
   <si>
@@ -285,9 +233,6 @@
     <t>DocVersion2</t>
   </si>
   <si>
-    <t>Chintan Shah</t>
-  </si>
-  <si>
     <t>Savings</t>
   </si>
   <si>
@@ -354,12 +299,6 @@
     <t>10</t>
   </si>
   <si>
-    <t>Tushar Shah</t>
-  </si>
-  <si>
-    <t>Khushbu Shah</t>
-  </si>
-  <si>
     <t>06/01/2019 01:10:00</t>
   </si>
   <si>
@@ -369,46 +308,106 @@
     <t>Timezone</t>
   </si>
   <si>
-    <t>999100000110</t>
-  </si>
-  <si>
-    <t>999100000111</t>
-  </si>
-  <si>
-    <t>999100000112</t>
-  </si>
-  <si>
-    <t>999100000113</t>
-  </si>
-  <si>
-    <t>Pradip</t>
-  </si>
-  <si>
-    <t>Jadhav</t>
-  </si>
-  <si>
-    <t>911781003</t>
-  </si>
-  <si>
-    <t>+17841253548</t>
-  </si>
-  <si>
-    <t>Pradip.jadhav@example.com</t>
-  </si>
-  <si>
-    <t>MID_200004</t>
-  </si>
-  <si>
-    <t>999100000114</t>
-  </si>
-  <si>
-    <t>Pradip Jadhav</t>
+    <t>Admin User</t>
+  </si>
+  <si>
+    <t>CustomerA@example.com</t>
+  </si>
+  <si>
+    <t>CustomerB@example.com</t>
+  </si>
+  <si>
+    <t>CustomerC@example.com</t>
+  </si>
+  <si>
+    <t>CustomerD@example.com</t>
+  </si>
+  <si>
+    <t>AccOwnership</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>shane</t>
+  </si>
+  <si>
+    <t>andrews</t>
+  </si>
+  <si>
+    <t>lynn</t>
+  </si>
+  <si>
+    <t>ramirez</t>
+  </si>
+  <si>
+    <t>caroline</t>
+  </si>
+  <si>
+    <t>carlson</t>
+  </si>
+  <si>
+    <t>louise</t>
+  </si>
+  <si>
+    <t>carter</t>
+  </si>
+  <si>
+    <t>911781015</t>
+  </si>
+  <si>
+    <t>911781016</t>
+  </si>
+  <si>
+    <t>911781017</t>
+  </si>
+  <si>
+    <t>911781018</t>
+  </si>
+  <si>
+    <t>MID_200015</t>
+  </si>
+  <si>
+    <t>MID_200016</t>
+  </si>
+  <si>
+    <t>MID_200017</t>
+  </si>
+  <si>
+    <t>MID_200018</t>
+  </si>
+  <si>
+    <t>+17810001015</t>
+  </si>
+  <si>
+    <t>+17810001016</t>
+  </si>
+  <si>
+    <t>+17810001017</t>
+  </si>
+  <si>
+    <t>+17810001018</t>
+  </si>
+  <si>
+    <t>999100000215</t>
+  </si>
+  <si>
+    <t>999100000216</t>
+  </si>
+  <si>
+    <t>999100000217</t>
+  </si>
+  <si>
+    <t>999100000218</t>
+  </si>
+  <si>
+    <t>999100000219</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -772,11 +771,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529D6B6E-4BCD-4333-A359-403F1D816D87}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +797,7 @@
     <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="21" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="23.7109375" bestFit="1" customWidth="1"/>
@@ -879,291 +878,284 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M2" s="1">
         <v>12008</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+      <c r="U2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M3" s="1">
         <v>12008</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M4" s="1">
         <v>12008</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M5" s="1">
         <v>12008</v>
       </c>
       <c r="N5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q5" s="1" t="s">
+      <c r="U5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="W5" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R2" r:id="rId1" xr:uid="{197C1862-2657-4B51-A0AD-493D5B1AB961}"/>
-    <hyperlink ref="R3" r:id="rId2" xr:uid="{C358DE7B-ECA7-4BBA-B620-2BC7A25D4B60}"/>
-    <hyperlink ref="R4" r:id="rId3" xr:uid="{3B7CE07F-5E5A-47F5-B460-44A0988A77A8}"/>
-    <hyperlink ref="R5" r:id="rId4" xr:uid="{62142599-8B21-4643-B883-A00C06ACE411}"/>
+    <hyperlink ref="R2" r:id="rId1"/>
+    <hyperlink ref="R3" r:id="rId2"/>
+    <hyperlink ref="R4" r:id="rId3"/>
+    <hyperlink ref="R5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -1171,41 +1163,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4410CAEF-738B-46B0-A005-2E917B7DBEFB}">
-  <dimension ref="A1:Y6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="13.7109375" customWidth="1"/>
-    <col min="18" max="18" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="13.7109375" customWidth="1"/>
+    <col min="19" max="19" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1216,353 +1207,371 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>83</v>
-      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M2" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="R2" s="1"/>
       <c r="S2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="V2" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="U3" s="1"/>
       <c r="V3" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1" t="s">
-        <v>98</v>
+        <v>79</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H4" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="R4" s="1"/>
       <c r="S4" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="V4" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="P5" s="1"/>
       <c r="Q5" s="1" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="V5" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>122</v>
+        <v>68</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M6" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="R6" s="1"/>
       <c r="S6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="V6" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>